<commit_message>
Add initial project structure and documentation for data processing
</commit_message>
<xml_diff>
--- a/data/congress/csv/2016FD.xlsx
+++ b/data/congress/csv/2016FD.xlsx
@@ -38366,7 +38366,7 @@
       </c>
       <c r="I683" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J683" t="inlineStr">
@@ -38419,7 +38419,7 @@
       </c>
       <c r="I684" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J684" t="inlineStr">
@@ -38472,7 +38472,7 @@
       </c>
       <c r="I685" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J685" t="inlineStr">
@@ -38525,7 +38525,7 @@
       </c>
       <c r="I686" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J686" t="inlineStr">
@@ -38578,7 +38578,7 @@
       </c>
       <c r="I687" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J687" t="inlineStr">
@@ -38631,7 +38631,7 @@
       </c>
       <c r="I688" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J688" t="inlineStr">
@@ -38684,7 +38684,7 @@
       </c>
       <c r="I689" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J689" t="inlineStr">
@@ -38737,7 +38737,7 @@
       </c>
       <c r="I690" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J690" t="inlineStr">
@@ -38790,7 +38790,7 @@
       </c>
       <c r="I691" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J691" t="inlineStr">
@@ -38843,7 +38843,7 @@
       </c>
       <c r="I692" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J692" t="inlineStr">
@@ -38896,7 +38896,7 @@
       </c>
       <c r="I693" t="inlineStr">
         <is>
-          <t>Spouse/DC</t>
+          <t>$1,000,001 - $5,000,000</t>
         </is>
       </c>
       <c r="J693" t="inlineStr">

</xml_diff>